<commit_message>
updated the UPD data mapping spreadsheet to facilitate database navigation
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Banshee_UDP_Mapping.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Banshee_UDP_Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="203">
   <si>
     <t>Device</t>
   </si>
@@ -454,9 +454,6 @@
   </si>
   <si>
     <t>Waveform</t>
-  </si>
-  <si>
-    <t>pu</t>
   </si>
   <si>
     <t>Relay Data</t>
@@ -1266,7 +1263,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1322,7 @@
         <v>140</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1375,16 +1372,16 @@
         <v>1</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>142</v>
@@ -1403,15 +1400,15 @@
         <v>10</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>142</v>
@@ -1430,15 +1427,15 @@
         <v>10</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>142</v>
@@ -1457,15 +1454,15 @@
         <v>100</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>142</v>
@@ -1484,15 +1481,15 @@
         <v>100</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>142</v>
@@ -1511,15 +1508,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>142</v>
@@ -1543,10 +1540,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>142</v>
@@ -1565,15 +1562,15 @@
         <v>100</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>142</v>
@@ -1592,15 +1589,15 @@
         <v>100</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>142</v>
@@ -1619,15 +1616,15 @@
         <v>100</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>142</v>
@@ -1646,15 +1643,15 @@
         <v>100</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>142</v>
@@ -1673,15 +1670,15 @@
         <v>100</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>142</v>
@@ -1700,15 +1697,15 @@
         <v>100</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>142</v>
@@ -1727,15 +1724,15 @@
         <v>100</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>142</v>
@@ -1754,15 +1751,15 @@
         <v>100</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>142</v>
@@ -1781,15 +1778,15 @@
         <v>100</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>142</v>
@@ -1808,15 +1805,15 @@
         <v>100</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>142</v>
@@ -1835,15 +1832,15 @@
         <v>1</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C23" s="35" t="s">
         <v>142</v>
@@ -1862,15 +1859,15 @@
         <v>1</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>142</v>
@@ -1894,10 +1891,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>160</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>142</v>
@@ -1921,10 +1918,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>142</v>
@@ -1943,15 +1940,15 @@
         <v>1</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>142</v>
@@ -1970,18 +1967,18 @@
         <v>1</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C28" s="39" t="s">
         <v>142</v>
@@ -2005,7 +2002,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>142</v>
@@ -2022,12 +2019,12 @@
       </c>
       <c r="G29" s="41"/>
       <c r="H29" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" s="45" t="s">
         <v>142</v>
@@ -2044,7 +2041,7 @@
       </c>
       <c r="G30" s="45"/>
       <c r="H30" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2060,7 +2057,7 @@
     </row>
     <row r="33" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E33" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F33" s="43">
         <f>SUM(F4:F32)</f>
@@ -2951,7 +2948,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>128</v>
@@ -2963,12 +2960,12 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -2982,7 +2979,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -3010,7 +3007,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>131</v>
@@ -3022,12 +3019,12 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>131</v>
@@ -3039,12 +3036,12 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>128</v>
@@ -3056,12 +3053,12 @@
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>131</v>
@@ -3073,12 +3070,12 @@
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>131</v>
@@ -3090,12 +3087,12 @@
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>131</v>
@@ -3107,12 +3104,12 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>131</v>
@@ -3124,7 +3121,7 @@
         <v>131</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated mapping to include ngchp updates
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Banshee_UDP_Mapping.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Banshee_UDP_Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="205">
   <si>
     <t>Device</t>
   </si>
@@ -543,9 +543,6 @@
     <t>Heat Recovered</t>
   </si>
   <si>
-    <t>CHP NOx</t>
-  </si>
-  <si>
     <t>CHP CO2</t>
   </si>
   <si>
@@ -625,6 +622,15 @@
   </si>
   <si>
     <t>None added to Banshee as of 10/27/2016</t>
+  </si>
+  <si>
+    <t>Boiler Nm^3/hr</t>
+  </si>
+  <si>
+    <t>Boiler lbm/hr CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel usage </t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,7 +1328,7 @@
         <v>140</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1340,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="24">
-        <f t="shared" ref="F4:F30" si="0">RIGHT(C4,2)/8*D4*E4*$C$1</f>
+        <f t="shared" ref="F4:F31" si="0">RIGHT(C4,2)/8*D4*E4*$C$1</f>
         <v>10</v>
       </c>
       <c r="G4" s="24"/>
@@ -1570,7 +1576,7 @@
         <v>170</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>142</v>
@@ -1597,7 +1603,7 @@
         <v>169</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>142</v>
@@ -1624,7 +1630,7 @@
         <v>169</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>142</v>
@@ -1643,7 +1649,7 @@
         <v>100</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1670,7 +1676,7 @@
         <v>100</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1678,7 +1684,7 @@
         <v>169</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>142</v>
@@ -1697,14 +1703,14 @@
         <v>100</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="10" t="s">
         <v>175</v>
       </c>
       <c r="C18" s="32" t="s">
@@ -1724,14 +1730,14 @@
         <v>100</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="16" t="s">
         <v>176</v>
       </c>
       <c r="C19" s="32" t="s">
@@ -1751,14 +1757,14 @@
         <v>100</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="10" t="s">
         <v>177</v>
       </c>
       <c r="C20" s="32" t="s">
@@ -1778,7 +1784,7 @@
         <v>100</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1786,7 +1792,7 @@
         <v>169</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>142</v>
@@ -1809,30 +1815,30 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="C22" s="35" t="s">
+      <c r="A22" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="35">
-        <v>1</v>
-      </c>
-      <c r="E22" s="35">
-        <v>1</v>
-      </c>
-      <c r="F22" s="36">
+      <c r="D22" s="32">
+        <v>1</v>
+      </c>
+      <c r="E22" s="33">
+        <v>1</v>
+      </c>
+      <c r="F22" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G22" s="35">
-        <v>1</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>188</v>
+      <c r="G22" s="32">
+        <v>100</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1840,7 +1846,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C23" s="35" t="s">
         <v>142</v>
@@ -1859,60 +1865,60 @@
         <v>1</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C24" s="25" t="s">
+      <c r="A24" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="25">
-        <v>1</v>
-      </c>
-      <c r="E24" s="25">
-        <v>1</v>
-      </c>
-      <c r="F24" s="26">
+      <c r="D24" s="35">
+        <v>1</v>
+      </c>
+      <c r="E24" s="35">
+        <v>1</v>
+      </c>
+      <c r="F24" s="36">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G24" s="25">
-        <v>1</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>131</v>
+      <c r="G24" s="35">
+        <v>1</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="37" t="s">
+      <c r="A25" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="37">
-        <v>1</v>
-      </c>
-      <c r="E25" s="37">
-        <v>3</v>
-      </c>
-      <c r="F25" s="38">
-        <f>RIGHT(C25,2)/8*D25*E25*$C$1</f>
-        <v>30</v>
-      </c>
-      <c r="G25" s="37">
-        <v>1000</v>
-      </c>
-      <c r="H25" s="19" t="s">
+      <c r="D25" s="25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G25" s="25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="14" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1921,7 +1927,7 @@
         <v>158</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>142</v>
@@ -1933,14 +1939,14 @@
         <v>3</v>
       </c>
       <c r="F26" s="38">
-        <f t="shared" si="0"/>
+        <f>RIGHT(C26,2)/8*D26*E26*$C$1</f>
         <v>30</v>
       </c>
       <c r="G26" s="37">
-        <v>1</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>186</v>
+        <v>1000</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1948,7 +1954,7 @@
         <v>158</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>142</v>
@@ -1967,101 +1973,128 @@
         <v>1</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="J27" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="37">
+        <v>1</v>
+      </c>
+      <c r="E28" s="37">
+        <v>3</v>
+      </c>
+      <c r="F28" s="38">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G28" s="37">
+        <v>1</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="J28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B29" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C29" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="39">
-        <v>1</v>
-      </c>
-      <c r="E28" s="39">
-        <v>1</v>
-      </c>
-      <c r="F28" s="40">
+      <c r="D29" s="39">
+        <v>1</v>
+      </c>
+      <c r="E29" s="39">
+        <v>1</v>
+      </c>
+      <c r="F29" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G28" s="39">
-        <v>1</v>
-      </c>
-      <c r="H28" s="21" t="s">
+      <c r="G29" s="39">
+        <v>1</v>
+      </c>
+      <c r="H29" s="21" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C30" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="D29" s="41">
-        <v>1</v>
-      </c>
-      <c r="E29" s="41">
-        <v>1</v>
-      </c>
-      <c r="F29" s="24">
+      <c r="D30" s="41">
+        <v>1</v>
+      </c>
+      <c r="E30" s="41">
+        <v>1</v>
+      </c>
+      <c r="F30" s="24">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G29" s="41"/>
-      <c r="H29" s="6" t="s">
+      <c r="G30" s="41"/>
+      <c r="H30" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+    <row r="31" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C31" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="D30" s="45">
-        <v>1</v>
-      </c>
-      <c r="E30" s="45">
-        <v>1</v>
-      </c>
-      <c r="F30" s="46">
+      <c r="D31" s="45">
+        <v>1</v>
+      </c>
+      <c r="E31" s="45">
+        <v>1</v>
+      </c>
+      <c r="F31" s="46">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="47" t="s">
+      <c r="G31" s="45"/>
+      <c r="H31" s="47" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E31" s="43">
-        <f>SUM(E6:E30)+E4+D5*E5</f>
-        <v>265</v>
-      </c>
-      <c r="F31" s="44"/>
-    </row>
     <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E32" s="44"/>
+      <c r="E32" s="43">
+        <f>SUM(E6:E31)+E4+D5*E5</f>
+        <v>266</v>
+      </c>
       <c r="F32" s="44"/>
     </row>
     <row r="33" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+    </row>
+    <row r="34" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E34" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="F33" s="43">
-        <f>SUM(F4:F32)</f>
-        <v>2650</v>
+      <c r="F34" s="43">
+        <f>SUM(F4:F33)</f>
+        <v>2660</v>
       </c>
     </row>
   </sheetData>
@@ -2948,7 +2981,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>128</v>
@@ -2960,12 +2993,12 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -2979,7 +3012,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -3007,7 +3040,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>131</v>
@@ -3019,12 +3052,12 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>131</v>
@@ -3036,12 +3069,12 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>128</v>
@@ -3053,12 +3086,12 @@
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>131</v>
@@ -3070,12 +3103,12 @@
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>131</v>
@@ -3087,12 +3120,12 @@
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>131</v>
@@ -3104,12 +3137,12 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>131</v>
@@ -3121,7 +3154,7 @@
         <v>131</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1) Fixed F4 Ess&PV relay settings 2) Modified sync check to reuse pll measurements already available in the model 3) Updated udp frame (unified frame for PHIL and Banshee)
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Banshee_UDP_Mapping.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Banshee_UDP_Mapping.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\re25624\Desktop\REPO_branch\DistributionSystems\SimulinkOpal\Banshee\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Relay Data - Order" sheetId="1" r:id="rId2"/>
     <sheet name="MiscData1 - Order" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -752,7 +747,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1065,6 +1060,26 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1087,26 +1102,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1157,11 +1152,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C37" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C37" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="A1:C37"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Load" dataDxfId="4"/>
-    <tableColumn id="2" name="Attribute" dataDxfId="3"/>
+    <tableColumn id="1" name="Load" dataDxfId="2"/>
+    <tableColumn id="2" name="Attribute" dataDxfId="1"/>
     <tableColumn id="3" name="Scale Factor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1211,7 +1206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1246,7 +1241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1457,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,11 +1580,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="23">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F6" s="21">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>590</v>
       </c>
       <c r="G6" s="23">
         <v>10</v>
@@ -1612,11 +1607,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="23">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F7" s="21">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>590</v>
       </c>
       <c r="G7" s="23">
         <v>10</v>
@@ -1639,11 +1634,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="23">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F8" s="21">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>590</v>
       </c>
       <c r="G8" s="23">
         <v>100</v>
@@ -1666,11 +1661,11 @@
         <v>1</v>
       </c>
       <c r="E9" s="23">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F9" s="21">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>590</v>
       </c>
       <c r="G9" s="23">
         <v>100</v>
@@ -1693,11 +1688,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="23">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F10" s="21">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>590</v>
       </c>
       <c r="G10" s="23">
         <v>1</v>
@@ -2371,11 +2366,11 @@
         <v>1</v>
       </c>
       <c r="E35" s="30">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F35" s="43">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="G35" s="30">
         <v>1</v>
@@ -2398,11 +2393,11 @@
         <v>1</v>
       </c>
       <c r="E36" s="30">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F36" s="43">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="G36" s="30">
         <v>1</v>
@@ -2971,7 +2966,7 @@
     <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E58" s="33">
         <f>SUM(E6:E57)+E4+D5*E5</f>
-        <v>331</v>
+        <v>400</v>
       </c>
       <c r="F58" s="34"/>
     </row>
@@ -2985,7 +2980,7 @@
       </c>
       <c r="F60" s="33">
         <f>SUM(F4:F59)</f>
-        <v>3310</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>